<commit_message>
Working on Receipt TAB
</commit_message>
<xml_diff>
--- a/src/main/java/com/agp/qa/testdata/TestData1.xlsx
+++ b/src/main/java/com/agp/qa/testdata/TestData1.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jignesh\Intellij Project\AGP\AGP\src\main\java\com\agp\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB4D91F-B1C3-4CDF-8A5A-4E0113D9CBE8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3A657A-F9A5-454B-9D9F-4046DECDE210}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9525" activeTab="1" xr2:uid="{8D0547BC-497C-496A-A490-9F7554F7CA35}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -202,14 +202,13 @@
     <t>Application No</t>
   </si>
   <si>
-    <t>JP30000166</t>
+    <t>JP30000177</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -626,41 +625,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8973B93E-C950-498E-BCBE-F2C95900CBBE}">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="Y9" sqref="Y9"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AF16" sqref="AF16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="5.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="26.0" collapsed="true"/>
-    <col min="8" max="9" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="32.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="28.7109375" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="35.5703125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="27" max="27" width="14.25" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="32.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="28.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="35.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -739,11 +738,11 @@
       <c r="Z1" t="s">
         <v>30</v>
       </c>
-      <c r="AA1" t="s" s="4">
+      <c r="AA1" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Commercial in One Flow
</commit_message>
<xml_diff>
--- a/src/main/java/com/agp/qa/testdata/TestData1.xlsx
+++ b/src/main/java/com/agp/qa/testdata/TestData1.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jignesh\Intellij Project\AGP\AGP\src\main\java\com\agp\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D116511-52E3-47B6-81B6-EDDB317423A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A068134-8980-40EE-9F0E-DA3551396EDD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9525" activeTab="1" xr2:uid="{8D0547BC-497C-496A-A490-9F7554F7CA35}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -271,19 +271,20 @@
     <t>Application No</t>
   </si>
   <si>
-    <t>JP30000182</t>
+    <t>JP30000195</t>
   </si>
   <si>
     <t>Consumer Number</t>
   </si>
   <si>
-    <t>JP30000090</t>
+    <t>JP30000097</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -702,50 +703,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8973B93E-C950-498E-BCBE-F2C95900CBBE}">
   <dimension ref="A1:AO2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AN1" sqref="AN1:AO2"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AO1" activeCellId="1" sqref="AN1:AN1048576 AO1:AO1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="32.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="28.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="35.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="13.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="14.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="14.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="36" width="14.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="18.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="14.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="15.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="5.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="8" max="9" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="32.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="35.5703125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="4" width="13.5703125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="4" width="14.7109375" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" style="4" width="13.5703125" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="4" width="14.5703125" collapsed="true"/>
+    <col min="31" max="36" customWidth="true" style="4" width="14.5703125" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" style="4" width="18.85546875" collapsed="true"/>
+    <col min="38" max="38" customWidth="true" style="4" width="14.5703125" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" style="4" width="15.42578125" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="14.25" collapsed="true"/>
+    <col min="41" max="41" width="18.01171875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -863,14 +864,14 @@
       <c r="AM1" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="AN1" s="5" t="s">
+      <c r="AN1" t="s" s="5">
         <v>80</v>
       </c>
-      <c r="AO1" s="6" t="s">
+      <c r="AO1" t="s" s="6">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>

</xml_diff>